<commit_message>
Finished prefabs & fixed dice
</commit_message>
<xml_diff>
--- a/Assets/Data/PropertyTycoonBoardData_StandardEdition.xlsx
+++ b/Assets/Data/PropertyTycoonBoardData_StandardEdition.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="111">
-  <si>
-    <t xml:space="preserve">Property Tycoon board data</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="111">
+  <si>
+    <t xml:space="preserve">Standard Edition</t>
   </si>
   <si>
     <t xml:space="preserve">If can be bought</t>
@@ -157,9 +157,6 @@
     <t xml:space="preserve">#000000</t>
   </si>
   <si>
-    <t xml:space="preserve">See notes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Weeping Angel</t>
   </si>
   <si>
@@ -194,6 +191,9 @@
   </si>
   <si>
     <t xml:space="preserve">Utilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#555555</t>
   </si>
   <si>
     <t xml:space="preserve">Wookie Hole</t>
@@ -556,10 +556,10 @@
   <dimension ref="A1:AD55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R13" activeCellId="0" sqref="R13"/>
+      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10"/>
@@ -1094,13 +1094,19 @@
       <c r="W10" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="X10" s="4" t="s">
-        <v>45</v>
+      <c r="X10" s="4" t="n">
+        <v>25</v>
       </c>
       <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
-      <c r="AB10" s="3"/>
+      <c r="Z10" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="AA10" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="AB10" s="4" t="n">
+        <v>200</v>
+      </c>
       <c r="AC10" s="3"/>
       <c r="AD10" s="3"/>
     </row>
@@ -1109,13 +1115,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" s="0" t="n">
         <f aca="false">HEX2DEC(MID($E11,2,2))/255</f>
@@ -1186,7 +1192,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F12" s="0" t="n">
         <f aca="false">HEX2DEC(MID($E12,2,2))/255</f>
@@ -1234,7 +1240,7 @@
         <v>33</v>
       </c>
       <c r="U12" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
@@ -1249,13 +1255,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F13" s="0" t="n">
         <f aca="false">HEX2DEC(MID($E13,2,2))/255</f>
@@ -1326,13 +1332,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>16</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F14" s="0" t="n">
         <f aca="false">HEX2DEC(MID($E14,2,2))/255</f>
@@ -1403,7 +1409,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F15" s="0" t="n">
         <f aca="false">HEX2DEC(MID($E15,2,2))/255</f>
@@ -1460,13 +1466,13 @@
         <v>12</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="E16" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>55</v>
       </c>
       <c r="F16" s="0" t="n">
         <f aca="false">HEX2DEC(MID($E16,2,2))/255</f>
@@ -1537,22 +1543,25 @@
         <v>13</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="E17" s="0" t="s">
         <v>57</v>
       </c>
       <c r="F17" s="0" t="n">
         <f aca="false">HEX2DEC(MID($E17,2,2))/255</f>
-        <v>0</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="G17" s="0" t="n">
         <f aca="false">HEX2DEC(MID($E17,4,2))/255</f>
-        <v>0</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="H17" s="0" t="n">
         <f aca="false">HEX2DEC(MID($E17,6,2))/255</f>
-        <v>0</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="J17" s="0" t="s">
         <v>33</v>
@@ -1587,11 +1596,13 @@
       <c r="W17" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="X17" s="4" t="s">
-        <v>45</v>
+      <c r="X17" s="4" t="n">
+        <v>4</v>
       </c>
       <c r="Y17" s="3"/>
-      <c r="Z17" s="3"/>
+      <c r="Z17" s="4" t="n">
+        <v>10</v>
+      </c>
       <c r="AA17" s="3"/>
       <c r="AB17" s="3"/>
       <c r="AC17" s="3"/>
@@ -1605,10 +1616,10 @@
         <v>58</v>
       </c>
       <c r="D18" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>55</v>
       </c>
       <c r="F18" s="0" t="n">
         <f aca="false">HEX2DEC(MID($E18,2,2))/255</f>
@@ -1682,10 +1693,10 @@
         <v>59</v>
       </c>
       <c r="D19" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>55</v>
       </c>
       <c r="F19" s="0" t="n">
         <f aca="false">HEX2DEC(MID($E19,2,2))/255</f>
@@ -1809,13 +1820,19 @@
       <c r="W20" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="X20" s="4" t="s">
-        <v>45</v>
+      <c r="X20" s="4" t="n">
+        <v>25</v>
       </c>
       <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
-      <c r="AA20" s="3"/>
-      <c r="AB20" s="3"/>
+      <c r="Z20" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="AA20" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="AB20" s="4" t="n">
+        <v>200</v>
+      </c>
       <c r="AC20" s="3"/>
       <c r="AD20" s="3"/>
     </row>
@@ -2255,7 +2272,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F27" s="0" t="n">
         <f aca="false">HEX2DEC(MID($E27,2,2))/255</f>
@@ -2303,7 +2320,7 @@
         <v>33</v>
       </c>
       <c r="U27" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
@@ -2525,13 +2542,19 @@
       <c r="W30" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="X30" s="4" t="s">
-        <v>45</v>
+      <c r="X30" s="4" t="n">
+        <v>25</v>
       </c>
       <c r="Y30" s="3"/>
-      <c r="Z30" s="3"/>
-      <c r="AA30" s="3"/>
-      <c r="AB30" s="3"/>
+      <c r="Z30" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="AA30" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="AB30" s="4" t="n">
+        <v>200</v>
+      </c>
       <c r="AC30" s="3"/>
       <c r="AD30" s="3"/>
     </row>
@@ -2697,19 +2720,22 @@
         <v>76</v>
       </c>
       <c r="D33" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>57</v>
       </c>
       <c r="F33" s="0" t="n">
         <f aca="false">HEX2DEC(MID($E33,2,2))/255</f>
-        <v>0</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="G33" s="0" t="n">
         <f aca="false">HEX2DEC(MID($E33,4,2))/255</f>
-        <v>0</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="H33" s="0" t="n">
         <f aca="false">HEX2DEC(MID($E33,6,2))/255</f>
-        <v>0</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="J33" s="0" t="s">
         <v>33</v>
@@ -2744,11 +2770,13 @@
       <c r="W33" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="X33" s="4" t="s">
-        <v>45</v>
+      <c r="X33" s="4" t="n">
+        <v>4</v>
       </c>
       <c r="Y33" s="3"/>
-      <c r="Z33" s="3"/>
+      <c r="Z33" s="4" t="n">
+        <v>10</v>
+      </c>
       <c r="AA33" s="3"/>
       <c r="AB33" s="3"/>
       <c r="AC33" s="3"/>
@@ -3243,13 +3271,19 @@
       <c r="W40" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="X40" s="4" t="s">
-        <v>45</v>
+      <c r="X40" s="4" t="n">
+        <v>25</v>
       </c>
       <c r="Y40" s="3"/>
-      <c r="Z40" s="3"/>
-      <c r="AA40" s="3"/>
-      <c r="AB40" s="3"/>
+      <c r="Z40" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="AA40" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="AB40" s="4" t="n">
+        <v>200</v>
+      </c>
       <c r="AC40" s="3"/>
       <c r="AD40" s="3"/>
     </row>
@@ -3258,7 +3292,7 @@
         <v>37</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>38</v>
@@ -3306,7 +3340,7 @@
         <v>33</v>
       </c>
       <c r="U41" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="X41" s="3"/>
       <c r="Y41" s="3"/>

</xml_diff>